<commit_message>
add new column what to Stundenprotokoll.xlsx
</commit_message>
<xml_diff>
--- a/Projektinfo/Stundenprotokoll.xlsx
+++ b/Projektinfo/Stundenprotokoll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\zbw\contact_manager\src\contact-manager\Projektinfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\Programming_Foundation_II\Projektarbeit\Projektinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043AE343-52F1-4FC9-BDAE-77B0DEEE1BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8DA202-2589-4FCA-8D4A-806CAEFF9942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A587525E-0DD3-41BC-BD44-5415FACA60EA}"/>
+    <workbookView xWindow="840" yWindow="1695" windowWidth="27750" windowHeight="13785" xr2:uid="{A587525E-0DD3-41BC-BD44-5415FACA60EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Patrick Nef " sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Cosimo Augustoni</t>
+  </si>
+  <si>
+    <t>Was?</t>
+  </si>
+  <si>
+    <t>Ausarbeitung Konzept, Analyse</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -121,6 +127,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,6 +178,9 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -186,9 +198,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -203,7 +212,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3EEA0226-D493-4917-BA6C-7B72C38FDF40}" name="Table13" displayName="Table13" ref="A4:D46" totalsRowCount="1" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3EEA0226-D493-4917-BA6C-7B72C38FDF40}" name="Table13" displayName="Table13" ref="A4:E46" totalsRowCount="1" headerRowDxfId="5">
+  <autoFilter ref="A4:E45" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{24B4437A-54AB-456A-8F4D-D2267BF202D7}" name="Datum" totalsRowLabel="Total" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{332A4454-D75C-42FE-A88B-0127FD945BC8}" name="Beginn"/>
+    <tableColumn id="3" xr3:uid="{C1F7D162-B241-4278-929E-19476FBBDF62}" name="Ende"/>
+    <tableColumn id="4" xr3:uid="{55CC84B2-B1D6-498A-B710-4C1B9B5D24ED}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
+    <tableColumn id="5" xr3:uid="{A1F3EB9C-CCF9-4C1E-9980-10979B87C2BA}" name="Was?"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C13F70F9-AA50-45AC-9FC4-D629FD96977B}" name="Table14" displayName="Table14" ref="A4:D46" totalsRowCount="1" headerRowDxfId="3">
   <autoFilter ref="A4:D45" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -211,25 +240,7 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{24B4437A-54AB-456A-8F4D-D2267BF202D7}" name="Datum" totalsRowLabel="Total" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{332A4454-D75C-42FE-A88B-0127FD945BC8}" name="Beginn"/>
-    <tableColumn id="3" xr3:uid="{C1F7D162-B241-4278-929E-19476FBBDF62}" name="Ende"/>
-    <tableColumn id="4" xr3:uid="{55CC84B2-B1D6-498A-B710-4C1B9B5D24ED}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C13F70F9-AA50-45AC-9FC4-D629FD96977B}" name="Table14" displayName="Table14" ref="A4:D46" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A4:D45" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECADE51F-0BE5-4E18-9708-DB4067A31F3A}" name="Datum" totalsRowLabel="Total" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{ECADE51F-0BE5-4E18-9708-DB4067A31F3A}" name="Datum" totalsRowLabel="Total" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{F77575EA-DE3E-4E65-A947-50684B707C1C}" name="Beginn"/>
     <tableColumn id="3" xr3:uid="{50C4ECC1-E4E5-400E-8B27-DB2EC8EF72C0}" name="Ende"/>
     <tableColumn id="4" xr3:uid="{A49F3DBD-E0FE-4C21-95F1-FC16F953169D}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
@@ -239,7 +250,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}" name="Table1" displayName="Table1" ref="A4:D46" totalsRowCount="1" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}" name="Table1" displayName="Table1" ref="A4:D46" totalsRowCount="1" headerRowDxfId="1">
   <autoFilter ref="A4:D45" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -247,7 +258,7 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5CAEBF57-CC40-40F3-9845-CFCDECBBB187}" name="Datum" totalsRowLabel="Total" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{5CAEBF57-CC40-40F3-9845-CFCDECBBB187}" name="Datum" totalsRowLabel="Total" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{1376C805-0C6A-4550-A447-3DA6D9157043}" name="Beginn"/>
     <tableColumn id="3" xr3:uid="{0F5A675D-D46C-413A-A881-4A4510951BDD}" name="Ende"/>
     <tableColumn id="4" xr3:uid="{911F8EDA-3C5F-446A-87F4-B942CFDDBD4E}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
@@ -555,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537DD32F-3B6D-41A7-8971-D5611D9EB56B}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +576,7 @@
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -603,6 +614,9 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -616,6 +630,9 @@
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4148C418-6D1C-4713-BE2C-8E34CDA13568}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
docs: updated stundenprotokoll und applikationsbeschreib
</commit_message>
<xml_diff>
--- a/Projektinfo/Stundenprotokoll.xlsx
+++ b/Projektinfo/Stundenprotokoll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Desktop\Programming_Foundation_II\Projektarbeit\Projektinfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\zbw\contact-manager\Projektinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940800A5-7715-482B-A338-512E242D827A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBB0B7A-C570-4818-AE3F-C4DC7FA969A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A587525E-0DD3-41BC-BD44-5415FACA60EA}"/>
+    <workbookView xWindow="40350" yWindow="1950" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{A587525E-0DD3-41BC-BD44-5415FACA60EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Patrick Nef " sheetId="4" r:id="rId1"/>
@@ -241,9 +241,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -295,6 +292,9 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -335,7 +335,7 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{24B4437A-54AB-456A-8F4D-D2267BF202D7}" name="Datum" totalsRowLabel="Total" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{24B4437A-54AB-456A-8F4D-D2267BF202D7}" name="Datum" totalsRowLabel="Total" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{332A4454-D75C-42FE-A88B-0127FD945BC8}" name="Beginn"/>
     <tableColumn id="3" xr3:uid="{C1F7D162-B241-4278-929E-19476FBBDF62}" name="Ende"/>
     <tableColumn id="4" xr3:uid="{55CC84B2-B1D6-498A-B710-4C1B9B5D24ED}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
@@ -346,7 +346,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C13F70F9-AA50-45AC-9FC4-D629FD96977B}" name="Table14" displayName="Table14" ref="A4:E47" totalsRowCount="1" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C13F70F9-AA50-45AC-9FC4-D629FD96977B}" name="Table14" displayName="Table14" ref="A4:E47" totalsRowCount="1" headerRowDxfId="6">
   <autoFilter ref="A4:E46" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -355,18 +355,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{ECADE51F-0BE5-4E18-9708-DB4067A31F3A}" name="Datum" totalsRowLabel="Total" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{ECADE51F-0BE5-4E18-9708-DB4067A31F3A}" name="Datum" totalsRowLabel="Total" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{F77575EA-DE3E-4E65-A947-50684B707C1C}" name="Beginn"/>
     <tableColumn id="3" xr3:uid="{50C4ECC1-E4E5-400E-8B27-DB2EC8EF72C0}" name="Ende"/>
     <tableColumn id="4" xr3:uid="{A49F3DBD-E0FE-4C21-95F1-FC16F953169D}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
-    <tableColumn id="5" xr3:uid="{1C36D830-1F03-429C-A742-C1250D4256C7}" name="Was?" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{1C36D830-1F03-429C-A742-C1250D4256C7}" name="Was?" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}" name="Table1" displayName="Table1" ref="A4:E46" totalsRowCount="1" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}" name="Table1" displayName="Table1" ref="A4:E46" totalsRowCount="1" headerRowDxfId="3">
   <autoFilter ref="A4:E45" xr:uid="{CA5EB60E-F8B9-4DC7-BC2E-2F4517F6186C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -375,11 +375,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5CAEBF57-CC40-40F3-9845-CFCDECBBB187}" name="Datum" totalsRowLabel="Total" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5CAEBF57-CC40-40F3-9845-CFCDECBBB187}" name="Datum" totalsRowLabel="Total" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{1376C805-0C6A-4550-A447-3DA6D9157043}" name="Beginn"/>
     <tableColumn id="3" xr3:uid="{0F5A675D-D46C-413A-A881-4A4510951BDD}" name="Ende"/>
     <tableColumn id="4" xr3:uid="{911F8EDA-3C5F-446A-87F4-B942CFDDBD4E}" name="Dauer (in Stunden)" totalsRowFunction="sum"/>
-    <tableColumn id="5" xr3:uid="{02BFF2CA-5EF4-44CF-984F-51E896538812}" name="Was?" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{02BFF2CA-5EF4-44CF-984F-51E896538812}" name="Was?" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -684,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537DD32F-3B6D-41A7-8971-D5611D9EB56B}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -1600,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFF7D92-3F7A-48AC-AE81-28EE3283910C}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,10 +1982,10 @@
         <v>0.75</v>
       </c>
       <c r="C43" s="4">
-        <v>0.875</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>43</v>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="D46">
         <f>SUBTOTAL(109,Table1[Dauer (in Stunden)])</f>
-        <v>37.5</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>